<commit_message>
template corrections and form.xls example corrections
</commit_message>
<xml_diff>
--- a/form.xlsx
+++ b/form.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Figueiredo\Desktop\Form\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael Figueiredo\Desktop\Form\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFF5EA2-8D28-4702-94F0-E3FD16EC5E13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76210A12-F834-4144-8D86-A2EBEE3C845C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="15375" windowHeight="7875" xr2:uid="{94016C9E-6D0B-476B-A5BD-31587DC00466}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>min</t>
   </si>
@@ -59,9 +59,6 @@
     <t>radio</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>type</t>
   </si>
   <si>
@@ -131,10 +128,10 @@
     <t>yes</t>
   </si>
   <si>
-    <t>', a, abc</t>
-  </si>
-  <si>
-    <t>Masculino,Femino,Outro</t>
+    <t>A,b, C</t>
+  </si>
+  <si>
+    <t>Male, Female, Other</t>
   </si>
 </sst>
 </file>
@@ -515,25 +512,25 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" t="s">
-        <v>10</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -542,55 +539,64 @@
         <v>1</v>
       </c>
       <c r="K1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
+      <c r="D2" t="s">
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -601,13 +607,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
@@ -615,48 +624,57 @@
       <c r="H5" t="s">
         <v>5</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>200</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>